<commit_message>
Portchannels and logical device build
</commit_message>
<xml_diff>
--- a/Spreadsheet.xlsx
+++ b/Spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\FXOSChassisOrchestrator\FXOSChassisOrchestrator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F641B01A-D52B-4571-B8F8-AED72847F8A0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D652366-D3AC-4F7B-BCAB-D91C268FA864}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FXOS DC1 Settings" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="182">
   <si>
     <t># DNS Configuration</t>
   </si>
@@ -494,6 +494,84 @@
   </si>
   <si>
     <t>Portchannel</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Member Interface</t>
+  </si>
+  <si>
+    <t>Ethernet1/4</t>
+  </si>
+  <si>
+    <t>Ethernet1/5</t>
+  </si>
+  <si>
+    <t>Ethernet1/6</t>
+  </si>
+  <si>
+    <t>Ethernet1/7</t>
+  </si>
+  <si>
+    <t>Ethernet1/8</t>
+  </si>
+  <si>
+    <t>Ethernet2/1</t>
+  </si>
+  <si>
+    <t>Ethernet2/2</t>
+  </si>
+  <si>
+    <t>Ethernet2/3</t>
+  </si>
+  <si>
+    <t>Ethernet2/4</t>
+  </si>
+  <si>
+    <t>Ethernet2/5</t>
+  </si>
+  <si>
+    <t>Ethernet2/6</t>
+  </si>
+  <si>
+    <t># Logical Device Configuration</t>
+  </si>
+  <si>
+    <t>ASA</t>
+  </si>
+  <si>
+    <t>Slot Number</t>
+  </si>
+  <si>
+    <t>Hostname</t>
+  </si>
+  <si>
+    <t>Software Version</t>
+  </si>
+  <si>
+    <t>ASA1</t>
+  </si>
+  <si>
+    <t>9.12.1</t>
+  </si>
+  <si>
+    <t>Management Interface</t>
+  </si>
+  <si>
+    <t>Portchannel30</t>
+  </si>
+  <si>
+    <t>Nameif</t>
+  </si>
+  <si>
+    <t>management</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>management link</t>
   </si>
 </sst>
 </file>
@@ -822,10 +900,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S58"/>
+  <dimension ref="A1:S59"/>
   <sheetViews>
     <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="G59" sqref="A52:G59"/>
+      <selection activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1629,7 +1707,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>148</v>
       </c>
@@ -1640,7 +1718,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>148</v>
       </c>
@@ -1651,7 +1729,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>7</v>
       </c>
@@ -1674,7 +1752,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>14</v>
       </c>
@@ -1697,7 +1775,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>14</v>
       </c>
@@ -1720,19 +1798,162 @@
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B56" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="L56" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="M56" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="N56" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="O56" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B57">
+        <v>10</v>
+      </c>
+      <c r="C57" t="s">
+        <v>17</v>
+      </c>
+      <c r="D57" t="s">
+        <v>18</v>
+      </c>
+      <c r="E57" t="s">
+        <v>19</v>
+      </c>
+      <c r="F57" t="s">
+        <v>20</v>
+      </c>
+      <c r="G57" t="s">
+        <v>75</v>
+      </c>
+      <c r="H57" t="s">
+        <v>15</v>
+      </c>
+      <c r="I57" t="s">
+        <v>21</v>
+      </c>
+      <c r="J57" t="s">
+        <v>22</v>
+      </c>
+      <c r="K57" t="s">
+        <v>158</v>
+      </c>
+      <c r="L57" t="s">
+        <v>159</v>
+      </c>
+      <c r="M57" t="s">
+        <v>160</v>
+      </c>
+      <c r="N57" t="s">
+        <v>161</v>
+      </c>
+      <c r="O57" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>155</v>
+      </c>
+      <c r="B58">
+        <v>20</v>
+      </c>
+      <c r="C58" t="s">
+        <v>17</v>
+      </c>
+      <c r="D58" t="s">
+        <v>18</v>
+      </c>
+      <c r="E58" t="s">
+        <v>19</v>
+      </c>
+      <c r="F58" t="s">
+        <v>20</v>
+      </c>
+      <c r="G58" t="s">
+        <v>75</v>
+      </c>
+      <c r="H58" t="s">
+        <v>163</v>
+      </c>
+      <c r="I58" t="s">
+        <v>164</v>
+      </c>
+      <c r="J58" t="s">
+        <v>165</v>
+      </c>
+      <c r="K58" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>155</v>
+      </c>
+      <c r="B59">
+        <v>30</v>
+      </c>
+      <c r="C59" t="s">
+        <v>17</v>
+      </c>
+      <c r="D59" t="s">
+        <v>18</v>
+      </c>
+      <c r="E59" t="s">
+        <v>19</v>
+      </c>
+      <c r="F59" t="s">
+        <v>20</v>
+      </c>
+      <c r="G59" t="s">
+        <v>75</v>
+      </c>
+      <c r="H59" t="s">
+        <v>167</v>
+      </c>
+      <c r="I59" t="s">
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -1775,10 +1996,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F317FE24-6344-4996-8321-5D3A5D44D647}">
-  <dimension ref="A1:S58"/>
+  <dimension ref="A1:S62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52:G59"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="G72" sqref="G72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1788,14 +2009,11 @@
     <col min="3" max="3" width="27.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="41.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.140625" customWidth="1"/>
+    <col min="9" max="10" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -2582,7 +2800,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>148</v>
       </c>
@@ -2593,7 +2811,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>148</v>
       </c>
@@ -2604,7 +2822,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>7</v>
       </c>
@@ -2627,7 +2845,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>14</v>
       </c>
@@ -2650,7 +2868,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>14</v>
       </c>
@@ -2673,19 +2891,208 @@
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B56" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="L56" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="M56" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="N56" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="O56" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B57">
+        <v>10</v>
+      </c>
+      <c r="C57" t="s">
+        <v>17</v>
+      </c>
+      <c r="D57" t="s">
+        <v>18</v>
+      </c>
+      <c r="E57" t="s">
+        <v>19</v>
+      </c>
+      <c r="F57" t="s">
+        <v>20</v>
+      </c>
+      <c r="G57" t="s">
+        <v>75</v>
+      </c>
+      <c r="H57" t="s">
+        <v>15</v>
+      </c>
+      <c r="I57" t="s">
+        <v>21</v>
+      </c>
+      <c r="J57" t="s">
+        <v>22</v>
+      </c>
+      <c r="K57" t="s">
+        <v>158</v>
+      </c>
+      <c r="L57" t="s">
+        <v>159</v>
+      </c>
+      <c r="M57" t="s">
+        <v>160</v>
+      </c>
+      <c r="N57" t="s">
+        <v>161</v>
+      </c>
+      <c r="O57" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>155</v>
+      </c>
+      <c r="B58">
+        <v>20</v>
+      </c>
+      <c r="C58" t="s">
+        <v>17</v>
+      </c>
+      <c r="D58" t="s">
+        <v>18</v>
+      </c>
+      <c r="E58" t="s">
+        <v>19</v>
+      </c>
+      <c r="F58" t="s">
+        <v>20</v>
+      </c>
+      <c r="G58" t="s">
+        <v>75</v>
+      </c>
+      <c r="H58" t="s">
+        <v>163</v>
+      </c>
+      <c r="I58" t="s">
+        <v>164</v>
+      </c>
+      <c r="J58" t="s">
+        <v>165</v>
+      </c>
+      <c r="K58" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>155</v>
+      </c>
+      <c r="B59">
+        <v>30</v>
+      </c>
+      <c r="C59" t="s">
+        <v>72</v>
+      </c>
+      <c r="D59" t="s">
+        <v>18</v>
+      </c>
+      <c r="E59" t="s">
+        <v>19</v>
+      </c>
+      <c r="F59" t="s">
+        <v>20</v>
+      </c>
+      <c r="G59" t="s">
+        <v>75</v>
+      </c>
+      <c r="H59" t="s">
+        <v>167</v>
+      </c>
+      <c r="I59" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>170</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="C62" t="s">
+        <v>174</v>
+      </c>
+      <c r="D62" t="s">
+        <v>175</v>
+      </c>
+      <c r="E62" t="s">
+        <v>177</v>
+      </c>
+      <c r="F62" t="s">
+        <v>179</v>
+      </c>
+      <c r="G62" t="s">
+        <v>181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ASA Logical Device added
</commit_message>
<xml_diff>
--- a/Spreadsheet.xlsx
+++ b/Spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\FXOSChassisOrchestrator\FXOSChassisOrchestrator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D652366-D3AC-4F7B-BCAB-D91C268FA864}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F78C0BD9-11A3-4849-BE50-B4845B9E642B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FXOS DC1 Settings" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="214">
   <si>
     <t># DNS Configuration</t>
   </si>
@@ -535,9 +535,6 @@
     <t>Ethernet2/6</t>
   </si>
   <si>
-    <t># Logical Device Configuration</t>
-  </si>
-  <si>
     <t>ASA</t>
   </si>
   <si>
@@ -559,9 +556,6 @@
     <t>Management Interface</t>
   </si>
   <si>
-    <t>Portchannel30</t>
-  </si>
-  <si>
     <t>Nameif</t>
   </si>
   <si>
@@ -571,7 +565,109 @@
     <t>Description</t>
   </si>
   <si>
-    <t>management link</t>
+    <t>Interface 1</t>
+  </si>
+  <si>
+    <t>inside</t>
+  </si>
+  <si>
+    <t>inside interface</t>
+  </si>
+  <si>
+    <t>Interface 2</t>
+  </si>
+  <si>
+    <t>Port-channel 30</t>
+  </si>
+  <si>
+    <t>Port-channel 10</t>
+  </si>
+  <si>
+    <t>Port-channel 20</t>
+  </si>
+  <si>
+    <t>Port-channel</t>
+  </si>
+  <si>
+    <t>outside</t>
+  </si>
+  <si>
+    <t>outside interface</t>
+  </si>
+  <si>
+    <t>Interface 3</t>
+  </si>
+  <si>
+    <t>Ethernet2/7</t>
+  </si>
+  <si>
+    <t>DMZ</t>
+  </si>
+  <si>
+    <t>DMZ interface</t>
+  </si>
+  <si>
+    <t>Interface 4</t>
+  </si>
+  <si>
+    <t>Ethernet2/8</t>
+  </si>
+  <si>
+    <t>DMZ2</t>
+  </si>
+  <si>
+    <t>DMZ2 interface</t>
+  </si>
+  <si>
+    <t>Firewall Mode</t>
+  </si>
+  <si>
+    <t>routed</t>
+  </si>
+  <si>
+    <t>Admin Password</t>
+  </si>
+  <si>
+    <t>cisco123</t>
+  </si>
+  <si>
+    <t>Management IP</t>
+  </si>
+  <si>
+    <t>192.168.1.1</t>
+  </si>
+  <si>
+    <t>Default Gateway</t>
+  </si>
+  <si>
+    <t>192.168.1.10</t>
+  </si>
+  <si>
+    <t>Subnet Mask</t>
+  </si>
+  <si>
+    <t>255.255.255.0</t>
+  </si>
+  <si>
+    <t>FTD</t>
+  </si>
+  <si>
+    <t># ASA Logical Device Configuration</t>
+  </si>
+  <si>
+    <t># FTD Logical Device Configuration</t>
+  </si>
+  <si>
+    <t>FTD1</t>
+  </si>
+  <si>
+    <t>192.168.1.20</t>
+  </si>
+  <si>
+    <t>6.2.3.83</t>
+  </si>
+  <si>
+    <t>management interface</t>
   </si>
 </sst>
 </file>
@@ -1996,10 +2092,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F317FE24-6344-4996-8321-5D3A5D44D647}">
-  <dimension ref="A1:S62"/>
+  <dimension ref="A1:X65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="G72" sqref="G72"/>
+    <sheetView tabSelected="1" topLeftCell="E43" workbookViewId="0">
+      <selection activeCell="H75" sqref="H75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2011,11 +2107,16 @@
     <col min="5" max="6" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -2800,7 +2901,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>148</v>
       </c>
@@ -2811,7 +2912,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>148</v>
       </c>
@@ -2822,7 +2923,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>7</v>
       </c>
@@ -2845,7 +2946,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>14</v>
       </c>
@@ -2868,7 +2969,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>14</v>
       </c>
@@ -2891,7 +2992,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>154</v>
       </c>
@@ -2938,9 +3039,9 @@
         <v>157</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>155</v>
+        <v>186</v>
       </c>
       <c r="B57">
         <v>10</v>
@@ -2975,19 +3076,10 @@
       <c r="L57" t="s">
         <v>159</v>
       </c>
-      <c r="M57" t="s">
-        <v>160</v>
-      </c>
-      <c r="N57" t="s">
-        <v>161</v>
-      </c>
-      <c r="O57" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>155</v>
+        <v>186</v>
       </c>
       <c r="B58">
         <v>20</v>
@@ -3020,9 +3112,9 @@
         <v>166</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>155</v>
+        <v>186</v>
       </c>
       <c r="B59">
         <v>30</v>
@@ -3049,50 +3141,282 @@
         <v>168</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="L61" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="M61" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="N61" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="O61" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="P61" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q61" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="R61" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="S61" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="T61" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="U61" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="V61" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="W61" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="X61" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>169</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="G61" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>170</v>
       </c>
       <c r="B62">
         <v>1</v>
       </c>
       <c r="C62" t="s">
+        <v>173</v>
+      </c>
+      <c r="D62" t="s">
         <v>174</v>
       </c>
-      <c r="D62" t="s">
+      <c r="E62" t="s">
+        <v>198</v>
+      </c>
+      <c r="F62" t="s">
+        <v>200</v>
+      </c>
+      <c r="G62" t="s">
+        <v>204</v>
+      </c>
+      <c r="H62" t="s">
+        <v>206</v>
+      </c>
+      <c r="I62" t="s">
+        <v>202</v>
+      </c>
+      <c r="J62" t="s">
+        <v>183</v>
+      </c>
+      <c r="K62" t="s">
+        <v>177</v>
+      </c>
+      <c r="L62" t="s">
+        <v>213</v>
+      </c>
+      <c r="M62" t="s">
+        <v>184</v>
+      </c>
+      <c r="N62" t="s">
+        <v>180</v>
+      </c>
+      <c r="O62" t="s">
+        <v>181</v>
+      </c>
+      <c r="P62" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>187</v>
+      </c>
+      <c r="R62" t="s">
+        <v>188</v>
+      </c>
+      <c r="S62" t="s">
+        <v>190</v>
+      </c>
+      <c r="T62" t="s">
+        <v>191</v>
+      </c>
+      <c r="U62" t="s">
+        <v>192</v>
+      </c>
+      <c r="V62" t="s">
+        <v>194</v>
+      </c>
+      <c r="W62" t="s">
+        <v>195</v>
+      </c>
+      <c r="X62" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="J64" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="E62" t="s">
+      <c r="K64" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="L64" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="M64" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="N64" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="O64" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="P64" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q64" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="R64" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="S64" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="T64" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="U64" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="V64" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="W64" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="X64" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>207</v>
+      </c>
+      <c r="B65">
+        <v>2</v>
+      </c>
+      <c r="C65" t="s">
+        <v>210</v>
+      </c>
+      <c r="D65" t="s">
+        <v>212</v>
+      </c>
+      <c r="E65" t="s">
+        <v>198</v>
+      </c>
+      <c r="F65" t="s">
+        <v>200</v>
+      </c>
+      <c r="G65" t="s">
+        <v>211</v>
+      </c>
+      <c r="H65" t="s">
+        <v>206</v>
+      </c>
+      <c r="I65" t="s">
+        <v>202</v>
+      </c>
+      <c r="J65" t="s">
+        <v>162</v>
+      </c>
+      <c r="K65" t="s">
         <v>177</v>
       </c>
-      <c r="F62" t="s">
-        <v>179</v>
-      </c>
-      <c r="G62" t="s">
+      <c r="L65" t="s">
+        <v>213</v>
+      </c>
+      <c r="M65" t="s">
+        <v>160</v>
+      </c>
+      <c r="N65" t="s">
+        <v>180</v>
+      </c>
+      <c r="O65" t="s">
         <v>181</v>
+      </c>
+      <c r="P65" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>187</v>
+      </c>
+      <c r="R65" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
if else statements removed
</commit_message>
<xml_diff>
--- a/Spreadsheet.xlsx
+++ b/Spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\FXOSChassisOrchestrator\FXOSChassisOrchestrator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C34CB49-2D30-4719-8FB9-4670AC08F7E1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D46AA8-7CC2-4CE4-9844-9C69F548A539}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FXOS DC1 Settings" sheetId="1" r:id="rId1"/>
@@ -1024,12 +1024,32 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="350" row="2">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{B5DB935A-F99B-4494-9958-0BD74B7EA678}">
+  <we:reference id="01cd1c88-25e9-4daa-b0ef-32dc541ed811" version="1.0.0.0" store="EXCatalog" storeType="EXCatalog"/>
+  <we:alternateReferences>
+    <we:reference id="WA200000068" version="1.0.0.0" store="en-US" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE66"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2460,7 +2480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F317FE24-6344-4996-8321-5D3A5D44D647}">
   <dimension ref="A1:AE66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>

</xml_diff>